<commit_message>
made some changes in utilities logging
</commit_message>
<xml_diff>
--- a/features/test_data/reports_file.xlsx
+++ b/features/test_data/reports_file.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
@@ -663,6 +663,21 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Verify Amazon User Login</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>